<commit_message>
Nova imagem + Controle de Tempo
</commit_message>
<xml_diff>
--- a/Controle-de-tempo.xlsx
+++ b/Controle-de-tempo.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10215"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
   <workbookPr date1904="1" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/leonardoamaral/Documents/GitHub/Automatizacao/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/16d1df2b2646901a/Documentos/GitHub/Automatizacao/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E50F906-144F-594E-B99D-9BAD18E2584F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="3" documentId="13_ncr:1_{4E50F906-144F-594E-B99D-9BAD18E2584F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5BCFD88C-C264-444B-9C5A-98EB1A116161}"/>
   <bookViews>
-    <workbookView xWindow="28800" yWindow="-11180" windowWidth="60160" windowHeight="33840" xr2:uid="{3FD58BC0-7166-A544-9D3F-4C0C6ADD0B8E}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{3FD58BC0-7166-A544-9D3F-4C0C6ADD0B8E}"/>
   </bookViews>
   <sheets>
     <sheet name="Controle de horas" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
         <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
       </xcalcf:calcFeatures>
@@ -34,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="19">
   <si>
     <t>Programador</t>
   </si>
@@ -1037,11 +1039,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3BA28EEB-0D8A-B34C-A5FE-30F0F9165161}">
   <dimension ref="A1:O244"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="16" style="3" customWidth="1"/>
     <col min="2" max="3" width="26" style="3" bestFit="1" customWidth="1"/>
@@ -1052,7 +1054,7 @@
     <col min="15" max="15" width="15.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -1072,7 +1074,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
         <v>2</v>
       </c>
@@ -1103,7 +1105,7 @@
       </c>
       <c r="N2" s="19"/>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A3" s="3" t="s">
         <v>2</v>
       </c>
@@ -1150,7 +1152,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A4" s="3" t="s">
         <v>2</v>
       </c>
@@ -1203,7 +1205,7 @@
         <v>-2.0833333333333259E-3</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A5" s="3" t="s">
         <v>1</v>
       </c>
@@ -1233,7 +1235,7 @@
       </c>
       <c r="J5" s="14">
         <f>E244</f>
-        <v>0.35</v>
+        <v>0.41249999999999998</v>
       </c>
       <c r="K5" s="14">
         <f>Tabela3[[#This Row],[Total Estimado]]/2</f>
@@ -1241,7 +1243,7 @@
       </c>
       <c r="L5" s="14">
         <f>SUMIFS($C$2:$C$200,$B$2:$B$200,"Semana 2",$A$2:$A$200,"Cesar")</f>
-        <v>0.10416666666666666</v>
+        <v>0.16666666666666666</v>
       </c>
       <c r="M5" s="14">
         <f>Tabela3[[#This Row],[Total Estimado]]/2</f>
@@ -1253,10 +1255,10 @@
       </c>
       <c r="O5" s="14">
         <f t="shared" ref="O5:O6" si="0">I5 - J5</f>
-        <v>0.48333333333333339</v>
-      </c>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
+        <v>0.42083333333333339</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A6" s="3" t="s">
         <v>1</v>
       </c>
@@ -1309,7 +1311,7 @@
         <v>0.83333333333333337</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A7" s="3" t="s">
         <v>1</v>
       </c>
@@ -1337,7 +1339,7 @@
       <c r="M7" s="1"/>
       <c r="N7" s="1"/>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A8" s="3" t="s">
         <v>1</v>
       </c>
@@ -1360,7 +1362,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A9" s="3" t="s">
         <v>2</v>
       </c>
@@ -1383,7 +1385,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A10" s="3" t="s">
         <v>1</v>
       </c>
@@ -1406,7 +1408,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A11" s="3" t="s">
         <v>2</v>
       </c>
@@ -1429,7 +1431,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A12" s="3" t="s">
         <v>2</v>
       </c>
@@ -1452,7 +1454,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A13" s="3" t="s">
         <v>1</v>
       </c>
@@ -1475,7 +1477,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A14" s="3" t="s">
         <v>2</v>
       </c>
@@ -1498,7 +1500,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A15" s="3" t="s">
         <v>2</v>
       </c>
@@ -1521,7 +1523,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A16" s="3" t="s">
         <v>1</v>
       </c>
@@ -1544,7 +1546,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A17" s="3" t="s">
         <v>2</v>
       </c>
@@ -1567,23 +1569,30 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B18" s="4"/>
-      <c r="C18" s="5"/>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A18" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C18" s="5">
+        <v>6.25E-2</v>
+      </c>
       <c r="D18" s="2">
         <f>IF(B18 = Fases!$A$2,Tabela2[[#This Row],[Tempo gasto]],0)</f>
         <v>0</v>
       </c>
       <c r="E18" s="2">
         <f>IF(B18 = Fases!$A$3,Tabela2[[#This Row],[Tempo gasto]],0)</f>
-        <v>0</v>
+        <v>6.25E-2</v>
       </c>
       <c r="F18" s="7">
         <f>IF(B18 = Fases!$A$4,Tabela2[[#This Row],[Tempo gasto]],0)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B19" s="4"/>
       <c r="C19" s="5"/>
       <c r="D19" s="2">
@@ -1599,7 +1608,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B20" s="4"/>
       <c r="C20" s="5"/>
       <c r="D20" s="2">
@@ -1615,7 +1624,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
       <c r="C21" s="5"/>
       <c r="D21" s="2">
         <f>IF(B21 = Fases!$A$2,Tabela2[[#This Row],[Tempo gasto]],0)</f>
@@ -1630,7 +1639,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
       <c r="C22" s="5"/>
       <c r="D22" s="2">
         <f>IF(B22 = Fases!$A$2,Tabela2[[#This Row],[Tempo gasto]],0)</f>
@@ -1645,7 +1654,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
       <c r="C23" s="5"/>
       <c r="D23" s="2">
         <f>IF(B23 = Fases!$A$2,Tabela2[[#This Row],[Tempo gasto]],0)</f>
@@ -1660,7 +1669,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
       <c r="C24" s="5"/>
       <c r="D24" s="2">
         <f>IF(B24 = Fases!$A$2,Tabela2[[#This Row],[Tempo gasto]],0)</f>
@@ -1675,7 +1684,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
       <c r="C25" s="5"/>
       <c r="D25" s="2">
         <f>IF(B25 = Fases!$A$2,Tabela2[[#This Row],[Tempo gasto]],0)</f>
@@ -1690,7 +1699,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
       <c r="C26" s="5"/>
       <c r="D26" s="2">
         <f>IF(B26 = Fases!$A$2,Tabela2[[#This Row],[Tempo gasto]],0)</f>
@@ -1705,7 +1714,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.35">
       <c r="C27" s="5"/>
       <c r="D27" s="2">
         <f>IF(B27 = Fases!$A$2,Tabela2[[#This Row],[Tempo gasto]],0)</f>
@@ -1720,7 +1729,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.35">
       <c r="C28" s="5"/>
       <c r="D28" s="2">
         <f>IF(B28 = Fases!$A$2,Tabela2[[#This Row],[Tempo gasto]],0)</f>
@@ -1735,7 +1744,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.35">
       <c r="C29" s="5"/>
       <c r="D29" s="2">
         <f>IF(B29 = Fases!$A$2,Tabela2[[#This Row],[Tempo gasto]],0)</f>
@@ -1750,7 +1759,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.35">
       <c r="C30" s="5"/>
       <c r="D30" s="2">
         <f>IF(B30 = Fases!$A$2,Tabela2[[#This Row],[Tempo gasto]],0)</f>
@@ -1765,7 +1774,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.35">
       <c r="C31" s="5"/>
       <c r="D31" s="2">
         <f>IF(B31 = Fases!$A$2,Tabela2[[#This Row],[Tempo gasto]],0)</f>
@@ -1780,7 +1789,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.35">
       <c r="C32" s="5"/>
       <c r="D32" s="2">
         <f>IF(B32 = Fases!$A$2,Tabela2[[#This Row],[Tempo gasto]],0)</f>
@@ -1795,7 +1804,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="33" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C33" s="5"/>
       <c r="D33" s="2">
         <f>IF(B33 = Fases!$A$2,Tabela2[[#This Row],[Tempo gasto]],0)</f>
@@ -1810,7 +1819,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="34" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C34" s="5"/>
       <c r="D34" s="2">
         <f>IF(B34 = Fases!$A$2,Tabela2[[#This Row],[Tempo gasto]],0)</f>
@@ -1825,7 +1834,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="35" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C35" s="5"/>
       <c r="D35" s="2">
         <f>IF(B35 = Fases!$A$2,Tabela2[[#This Row],[Tempo gasto]],0)</f>
@@ -1840,7 +1849,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="36" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C36" s="5"/>
       <c r="D36" s="2">
         <f>IF(B36 = Fases!$A$2,Tabela2[[#This Row],[Tempo gasto]],0)</f>
@@ -1855,7 +1864,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="37" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C37" s="5"/>
       <c r="D37" s="2">
         <f>IF(B37 = Fases!$A$2,Tabela2[[#This Row],[Tempo gasto]],0)</f>
@@ -1870,7 +1879,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="38" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C38" s="5"/>
       <c r="D38" s="2">
         <f>IF(B38 = Fases!$A$2,Tabela2[[#This Row],[Tempo gasto]],0)</f>
@@ -1885,7 +1894,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="39" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C39" s="5"/>
       <c r="D39" s="2">
         <f>IF(B39 = Fases!$A$2,Tabela2[[#This Row],[Tempo gasto]],0)</f>
@@ -1900,7 +1909,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="40" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C40" s="5"/>
       <c r="D40" s="2">
         <f>IF(B40 = Fases!$A$2,Tabela2[[#This Row],[Tempo gasto]],0)</f>
@@ -1915,7 +1924,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="41" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C41" s="5"/>
       <c r="D41" s="2">
         <f>IF(B41 = Fases!$A$2,Tabela2[[#This Row],[Tempo gasto]],0)</f>
@@ -1930,7 +1939,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="42" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C42" s="5"/>
       <c r="D42" s="2">
         <f>IF(B42 = Fases!$A$2,Tabela2[[#This Row],[Tempo gasto]],0)</f>
@@ -1945,7 +1954,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="43" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C43" s="5"/>
       <c r="D43" s="2">
         <f>IF(B43 = Fases!$A$2,Tabela2[[#This Row],[Tempo gasto]],0)</f>
@@ -1960,7 +1969,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="44" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C44" s="5"/>
       <c r="D44" s="2">
         <f>IF(B44 = Fases!$A$2,Tabela2[[#This Row],[Tempo gasto]],0)</f>
@@ -1975,7 +1984,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="45" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C45" s="5"/>
       <c r="D45" s="2">
         <f>IF(B45 = Fases!$A$2,Tabela2[[#This Row],[Tempo gasto]],0)</f>
@@ -1990,7 +1999,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="46" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C46" s="5"/>
       <c r="D46" s="2">
         <f>IF(B46 = Fases!$A$2,Tabela2[[#This Row],[Tempo gasto]],0)</f>
@@ -2005,7 +2014,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="47" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C47" s="5"/>
       <c r="D47" s="2">
         <f>IF(B47 = Fases!$A$2,Tabela2[[#This Row],[Tempo gasto]],0)</f>
@@ -2020,7 +2029,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="48" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C48" s="5"/>
       <c r="D48" s="2">
         <f>IF(B48 = Fases!$A$2,Tabela2[[#This Row],[Tempo gasto]],0)</f>
@@ -2035,7 +2044,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="49" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C49" s="5"/>
       <c r="D49" s="2">
         <f>IF(B49 = Fases!$A$2,Tabela2[[#This Row],[Tempo gasto]],0)</f>
@@ -2050,7 +2059,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="50" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C50" s="5"/>
       <c r="D50" s="2">
         <f>IF(B50 = Fases!$A$2,Tabela2[[#This Row],[Tempo gasto]],0)</f>
@@ -2065,7 +2074,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="51" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C51" s="5"/>
       <c r="D51" s="2">
         <f>IF(B51 = Fases!$A$2,Tabela2[[#This Row],[Tempo gasto]],0)</f>
@@ -2080,7 +2089,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="52" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C52" s="5"/>
       <c r="D52" s="2">
         <f>IF(B52 = Fases!$A$2,Tabela2[[#This Row],[Tempo gasto]],0)</f>
@@ -2095,7 +2104,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="53" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C53" s="5"/>
       <c r="D53" s="2">
         <f>IF(B53 = Fases!$A$2,Tabela2[[#This Row],[Tempo gasto]],0)</f>
@@ -2110,7 +2119,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="54" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C54" s="5"/>
       <c r="D54" s="2">
         <f>IF(B54 = Fases!$A$2,Tabela2[[#This Row],[Tempo gasto]],0)</f>
@@ -2125,7 +2134,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="55" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C55" s="5"/>
       <c r="D55" s="2">
         <f>IF(B55 = Fases!$A$2,Tabela2[[#This Row],[Tempo gasto]],0)</f>
@@ -2140,7 +2149,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="56" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C56" s="5"/>
       <c r="D56" s="2">
         <f>IF(B56 = Fases!$A$2,Tabela2[[#This Row],[Tempo gasto]],0)</f>
@@ -2155,7 +2164,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="57" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C57" s="5"/>
       <c r="D57" s="2">
         <f>IF(B57 = Fases!$A$2,Tabela2[[#This Row],[Tempo gasto]],0)</f>
@@ -2170,7 +2179,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="58" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C58" s="5"/>
       <c r="D58" s="2">
         <f>IF(B58 = Fases!$A$2,Tabela2[[#This Row],[Tempo gasto]],0)</f>
@@ -2185,7 +2194,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="59" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C59" s="5"/>
       <c r="D59" s="2">
         <f>IF(B59 = Fases!$A$2,Tabela2[[#This Row],[Tempo gasto]],0)</f>
@@ -2200,7 +2209,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="60" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C60" s="5"/>
       <c r="D60" s="2">
         <f>IF(B60 = Fases!$A$2,Tabela2[[#This Row],[Tempo gasto]],0)</f>
@@ -2215,7 +2224,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="61" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C61" s="5"/>
       <c r="D61" s="2">
         <f>IF(B61 = Fases!$A$2,Tabela2[[#This Row],[Tempo gasto]],0)</f>
@@ -2230,7 +2239,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="62" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C62" s="5"/>
       <c r="D62" s="2">
         <f>IF(B62 = Fases!$A$2,Tabela2[[#This Row],[Tempo gasto]],0)</f>
@@ -2245,7 +2254,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="63" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C63" s="5"/>
       <c r="D63" s="2">
         <f>IF(B63 = Fases!$A$2,Tabela2[[#This Row],[Tempo gasto]],0)</f>
@@ -2260,7 +2269,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="64" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C64" s="5"/>
       <c r="D64" s="2">
         <f>IF(B64 = Fases!$A$2,Tabela2[[#This Row],[Tempo gasto]],0)</f>
@@ -2275,7 +2284,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="65" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C65" s="5"/>
       <c r="D65" s="2">
         <f>IF(B65 = Fases!$A$2,Tabela2[[#This Row],[Tempo gasto]],0)</f>
@@ -2290,7 +2299,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="66" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C66" s="5"/>
       <c r="D66" s="2">
         <f>IF(B66 = Fases!$A$2,Tabela2[[#This Row],[Tempo gasto]],0)</f>
@@ -2305,7 +2314,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="67" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C67" s="5"/>
       <c r="D67" s="2">
         <f>IF(B67 = Fases!$A$2,Tabela2[[#This Row],[Tempo gasto]],0)</f>
@@ -2320,7 +2329,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="68" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C68" s="5"/>
       <c r="D68" s="2">
         <f>IF(B68 = Fases!$A$2,Tabela2[[#This Row],[Tempo gasto]],0)</f>
@@ -2335,7 +2344,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="69" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C69" s="5"/>
       <c r="D69" s="2">
         <f>IF(B69 = Fases!$A$2,Tabela2[[#This Row],[Tempo gasto]],0)</f>
@@ -2350,7 +2359,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="70" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C70" s="5"/>
       <c r="D70" s="2">
         <f>IF(B70 = Fases!$A$2,Tabela2[[#This Row],[Tempo gasto]],0)</f>
@@ -2365,7 +2374,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="71" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C71" s="5"/>
       <c r="D71" s="2">
         <f>IF(B71 = Fases!$A$2,Tabela2[[#This Row],[Tempo gasto]],0)</f>
@@ -2380,7 +2389,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="72" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C72" s="5"/>
       <c r="D72" s="2">
         <f>IF(B72 = Fases!$A$2,Tabela2[[#This Row],[Tempo gasto]],0)</f>
@@ -2395,7 +2404,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="73" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="73" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C73" s="5"/>
       <c r="D73" s="2">
         <f>IF(B73 = Fases!$A$2,Tabela2[[#This Row],[Tempo gasto]],0)</f>
@@ -2410,7 +2419,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="74" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="74" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C74" s="5"/>
       <c r="D74" s="2">
         <f>IF(B74 = Fases!$A$2,Tabela2[[#This Row],[Tempo gasto]],0)</f>
@@ -2425,7 +2434,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="75" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="75" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C75" s="5"/>
       <c r="D75" s="2">
         <f>IF(B75 = Fases!$A$2,Tabela2[[#This Row],[Tempo gasto]],0)</f>
@@ -2440,7 +2449,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="76" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="76" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C76" s="5"/>
       <c r="D76" s="2">
         <f>IF(B76 = Fases!$A$2,Tabela2[[#This Row],[Tempo gasto]],0)</f>
@@ -2455,7 +2464,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="77" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="77" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C77" s="5"/>
       <c r="D77" s="2">
         <f>IF(B77 = Fases!$A$2,Tabela2[[#This Row],[Tempo gasto]],0)</f>
@@ -2470,7 +2479,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="78" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="78" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C78" s="5"/>
       <c r="D78" s="2">
         <f>IF(B78 = Fases!$A$2,Tabela2[[#This Row],[Tempo gasto]],0)</f>
@@ -2485,7 +2494,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="79" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="79" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C79" s="5"/>
       <c r="D79" s="2">
         <f>IF(B79 = Fases!$A$2,Tabela2[[#This Row],[Tempo gasto]],0)</f>
@@ -2500,7 +2509,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="80" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="80" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C80" s="5"/>
       <c r="D80" s="2">
         <f>IF(B80 = Fases!$A$2,Tabela2[[#This Row],[Tempo gasto]],0)</f>
@@ -2515,7 +2524,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="81" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="81" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C81" s="5"/>
       <c r="D81" s="2">
         <f>IF(B81 = Fases!$A$2,Tabela2[[#This Row],[Tempo gasto]],0)</f>
@@ -2530,7 +2539,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="82" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="82" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C82" s="5"/>
       <c r="D82" s="2">
         <f>IF(B82 = Fases!$A$2,Tabela2[[#This Row],[Tempo gasto]],0)</f>
@@ -2545,7 +2554,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="83" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="83" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C83" s="5"/>
       <c r="D83" s="2">
         <f>IF(B83 = Fases!$A$2,Tabela2[[#This Row],[Tempo gasto]],0)</f>
@@ -2560,7 +2569,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="84" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="84" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C84" s="5"/>
       <c r="D84" s="2">
         <f>IF(B84 = Fases!$A$2,Tabela2[[#This Row],[Tempo gasto]],0)</f>
@@ -2575,7 +2584,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="85" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="85" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C85" s="5"/>
       <c r="D85" s="2">
         <f>IF(B85 = Fases!$A$2,Tabela2[[#This Row],[Tempo gasto]],0)</f>
@@ -2590,7 +2599,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="86" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="86" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C86" s="5"/>
       <c r="D86" s="2">
         <f>IF(B86 = Fases!$A$2,Tabela2[[#This Row],[Tempo gasto]],0)</f>
@@ -2605,7 +2614,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="87" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="87" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C87" s="5"/>
       <c r="D87" s="2">
         <f>IF(B87 = Fases!$A$2,Tabela2[[#This Row],[Tempo gasto]],0)</f>
@@ -2620,7 +2629,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="88" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="88" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C88" s="5"/>
       <c r="D88" s="2">
         <f>IF(B88 = Fases!$A$2,Tabela2[[#This Row],[Tempo gasto]],0)</f>
@@ -2635,7 +2644,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="89" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="89" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C89" s="5"/>
       <c r="D89" s="2">
         <f>IF(B89 = Fases!$A$2,Tabela2[[#This Row],[Tempo gasto]],0)</f>
@@ -2650,7 +2659,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="90" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="90" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C90" s="5"/>
       <c r="D90" s="2">
         <f>IF(B90 = Fases!$A$2,Tabela2[[#This Row],[Tempo gasto]],0)</f>
@@ -2665,7 +2674,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="91" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="91" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C91" s="5"/>
       <c r="D91" s="2">
         <f>IF(B91 = Fases!$A$2,Tabela2[[#This Row],[Tempo gasto]],0)</f>
@@ -2680,7 +2689,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="92" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="92" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C92" s="5"/>
       <c r="D92" s="2">
         <f>IF(B92 = Fases!$A$2,Tabela2[[#This Row],[Tempo gasto]],0)</f>
@@ -2695,7 +2704,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="93" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="93" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C93" s="5"/>
       <c r="D93" s="2">
         <f>IF(B93 = Fases!$A$2,Tabela2[[#This Row],[Tempo gasto]],0)</f>
@@ -2710,7 +2719,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="94" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="94" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C94" s="5"/>
       <c r="D94" s="2">
         <f>IF(B94 = Fases!$A$2,Tabela2[[#This Row],[Tempo gasto]],0)</f>
@@ -2725,7 +2734,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="95" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="95" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C95" s="5"/>
       <c r="D95" s="2">
         <f>IF(B95 = Fases!$A$2,Tabela2[[#This Row],[Tempo gasto]],0)</f>
@@ -2740,7 +2749,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="96" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="96" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C96" s="5"/>
       <c r="D96" s="2">
         <f>IF(B96 = Fases!$A$2,Tabela2[[#This Row],[Tempo gasto]],0)</f>
@@ -2755,7 +2764,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="97" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="97" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C97" s="5"/>
       <c r="D97" s="2">
         <f>IF(B97 = Fases!$A$2,Tabela2[[#This Row],[Tempo gasto]],0)</f>
@@ -2770,7 +2779,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="98" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="98" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C98" s="5"/>
       <c r="D98" s="2">
         <f>IF(B98 = Fases!$A$2,Tabela2[[#This Row],[Tempo gasto]],0)</f>
@@ -2785,7 +2794,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="99" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="99" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C99" s="5"/>
       <c r="D99" s="2">
         <f>IF(B99 = Fases!$A$2,Tabela2[[#This Row],[Tempo gasto]],0)</f>
@@ -2800,7 +2809,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="100" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="100" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C100" s="5"/>
       <c r="D100" s="2">
         <f>IF(B100 = Fases!$A$2,Tabela2[[#This Row],[Tempo gasto]],0)</f>
@@ -2815,7 +2824,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="101" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="101" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C101" s="5"/>
       <c r="D101" s="2">
         <f>IF(B101 = Fases!$A$2,Tabela2[[#This Row],[Tempo gasto]],0)</f>
@@ -2830,7 +2839,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="102" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="102" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C102" s="5"/>
       <c r="D102" s="2">
         <f>IF(B102 = Fases!$A$2,Tabela2[[#This Row],[Tempo gasto]],0)</f>
@@ -2845,7 +2854,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="103" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="103" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C103" s="5"/>
       <c r="D103" s="2">
         <f>IF(B103 = Fases!$A$2,Tabela2[[#This Row],[Tempo gasto]],0)</f>
@@ -2860,7 +2869,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="104" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="104" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C104" s="5"/>
       <c r="D104" s="2">
         <f>IF(B104 = Fases!$A$2,Tabela2[[#This Row],[Tempo gasto]],0)</f>
@@ -2875,7 +2884,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="105" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="105" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C105" s="5"/>
       <c r="D105" s="2">
         <f>IF(B105 = Fases!$A$2,Tabela2[[#This Row],[Tempo gasto]],0)</f>
@@ -2890,7 +2899,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="106" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="106" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C106" s="5"/>
       <c r="D106" s="2">
         <f>IF(B106 = Fases!$A$2,Tabela2[[#This Row],[Tempo gasto]],0)</f>
@@ -2905,7 +2914,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="107" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="107" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C107" s="5"/>
       <c r="D107" s="2">
         <f>IF(B107 = Fases!$A$2,Tabela2[[#This Row],[Tempo gasto]],0)</f>
@@ -2920,7 +2929,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="108" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="108" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C108" s="5"/>
       <c r="D108" s="2">
         <f>IF(B108 = Fases!$A$2,Tabela2[[#This Row],[Tempo gasto]],0)</f>
@@ -2935,7 +2944,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="109" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="109" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C109" s="5"/>
       <c r="D109" s="2">
         <f>IF(B109 = Fases!$A$2,Tabela2[[#This Row],[Tempo gasto]],0)</f>
@@ -2950,7 +2959,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="110" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="110" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C110" s="5"/>
       <c r="D110" s="2">
         <f>IF(B110 = Fases!$A$2,Tabela2[[#This Row],[Tempo gasto]],0)</f>
@@ -2965,7 +2974,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="111" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="111" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C111" s="5"/>
       <c r="D111" s="2">
         <f>IF(B111 = Fases!$A$2,Tabela2[[#This Row],[Tempo gasto]],0)</f>
@@ -2980,7 +2989,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="112" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="112" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C112" s="5"/>
       <c r="D112" s="2">
         <f>IF(B112 = Fases!$A$2,Tabela2[[#This Row],[Tempo gasto]],0)</f>
@@ -2995,7 +3004,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="113" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="113" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C113" s="5"/>
       <c r="D113" s="2">
         <f>IF(B113 = Fases!$A$2,Tabela2[[#This Row],[Tempo gasto]],0)</f>
@@ -3010,7 +3019,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="114" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="114" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C114" s="5"/>
       <c r="D114" s="2">
         <f>IF(B114 = Fases!$A$2,Tabela2[[#This Row],[Tempo gasto]],0)</f>
@@ -3025,7 +3034,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="115" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="115" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C115" s="5"/>
       <c r="D115" s="2">
         <f>IF(B115 = Fases!$A$2,Tabela2[[#This Row],[Tempo gasto]],0)</f>
@@ -3040,7 +3049,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="116" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="116" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C116" s="5"/>
       <c r="D116" s="2">
         <f>IF(B116 = Fases!$A$2,Tabela2[[#This Row],[Tempo gasto]],0)</f>
@@ -3055,7 +3064,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="117" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="117" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C117" s="5"/>
       <c r="D117" s="2">
         <f>IF(B117 = Fases!$A$2,Tabela2[[#This Row],[Tempo gasto]],0)</f>
@@ -3070,7 +3079,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="118" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="118" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C118" s="5"/>
       <c r="D118" s="2">
         <f>IF(B118 = Fases!$A$2,Tabela2[[#This Row],[Tempo gasto]],0)</f>
@@ -3085,7 +3094,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="119" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="119" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C119" s="5"/>
       <c r="D119" s="2">
         <f>IF(B119 = Fases!$A$2,Tabela2[[#This Row],[Tempo gasto]],0)</f>
@@ -3100,7 +3109,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="120" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="120" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C120" s="5"/>
       <c r="D120" s="2">
         <f>IF(B120 = Fases!$A$2,Tabela2[[#This Row],[Tempo gasto]],0)</f>
@@ -3115,7 +3124,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="121" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="121" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C121" s="5"/>
       <c r="D121" s="2">
         <f>IF(B121 = Fases!$A$2,Tabela2[[#This Row],[Tempo gasto]],0)</f>
@@ -3130,7 +3139,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="122" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="122" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C122" s="5"/>
       <c r="D122" s="2">
         <f>IF(B122 = Fases!$A$2,Tabela2[[#This Row],[Tempo gasto]],0)</f>
@@ -3145,7 +3154,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="123" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="123" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C123" s="5"/>
       <c r="D123" s="2">
         <f>IF(B123 = Fases!$A$2,Tabela2[[#This Row],[Tempo gasto]],0)</f>
@@ -3160,7 +3169,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="124" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="124" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C124" s="5"/>
       <c r="D124" s="2">
         <f>IF(B124 = Fases!$A$2,Tabela2[[#This Row],[Tempo gasto]],0)</f>
@@ -3175,7 +3184,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="125" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="125" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C125" s="5"/>
       <c r="D125" s="2">
         <f>IF(B125 = Fases!$A$2,Tabela2[[#This Row],[Tempo gasto]],0)</f>
@@ -3190,7 +3199,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="126" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="126" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C126" s="5"/>
       <c r="D126" s="2">
         <f>IF(B126 = Fases!$A$2,Tabela2[[#This Row],[Tempo gasto]],0)</f>
@@ -3205,7 +3214,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="127" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="127" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C127" s="5"/>
       <c r="D127" s="2">
         <f>IF(B127 = Fases!$A$2,Tabela2[[#This Row],[Tempo gasto]],0)</f>
@@ -3220,7 +3229,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="128" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="128" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C128" s="5"/>
       <c r="D128" s="2">
         <f>IF(B128 = Fases!$A$2,Tabela2[[#This Row],[Tempo gasto]],0)</f>
@@ -3235,7 +3244,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="129" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="129" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C129" s="5"/>
       <c r="D129" s="2">
         <f>IF(B129 = Fases!$A$2,Tabela2[[#This Row],[Tempo gasto]],0)</f>
@@ -3250,7 +3259,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="130" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="130" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C130" s="5"/>
       <c r="D130" s="2">
         <f>IF(B130 = Fases!$A$2,Tabela2[[#This Row],[Tempo gasto]],0)</f>
@@ -3265,7 +3274,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="131" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="131" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C131" s="5"/>
       <c r="D131" s="2">
         <f>IF(B131 = Fases!$A$2,Tabela2[[#This Row],[Tempo gasto]],0)</f>
@@ -3280,7 +3289,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="132" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="132" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C132" s="5"/>
       <c r="D132" s="2">
         <f>IF(B132 = Fases!$A$2,Tabela2[[#This Row],[Tempo gasto]],0)</f>
@@ -3295,7 +3304,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="133" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="133" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C133" s="5"/>
       <c r="D133" s="2">
         <f>IF(B133 = Fases!$A$2,Tabela2[[#This Row],[Tempo gasto]],0)</f>
@@ -3310,7 +3319,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="134" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="134" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C134" s="5"/>
       <c r="D134" s="2">
         <f>IF(B134 = Fases!$A$2,Tabela2[[#This Row],[Tempo gasto]],0)</f>
@@ -3325,7 +3334,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="135" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="135" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C135" s="5"/>
       <c r="D135" s="2">
         <f>IF(B135 = Fases!$A$2,Tabela2[[#This Row],[Tempo gasto]],0)</f>
@@ -3340,7 +3349,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="136" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="136" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C136" s="5"/>
       <c r="D136" s="2">
         <f>IF(B136 = Fases!$A$2,Tabela2[[#This Row],[Tempo gasto]],0)</f>
@@ -3355,7 +3364,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="137" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="137" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C137" s="5"/>
       <c r="D137" s="2">
         <f>IF(B137 = Fases!$A$2,Tabela2[[#This Row],[Tempo gasto]],0)</f>
@@ -3370,7 +3379,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="138" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="138" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C138" s="5"/>
       <c r="D138" s="2">
         <f>IF(B138 = Fases!$A$2,Tabela2[[#This Row],[Tempo gasto]],0)</f>
@@ -3385,7 +3394,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="139" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="139" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C139" s="5"/>
       <c r="D139" s="2">
         <f>IF(B139 = Fases!$A$2,Tabela2[[#This Row],[Tempo gasto]],0)</f>
@@ -3400,7 +3409,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="140" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="140" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C140" s="5"/>
       <c r="D140" s="2">
         <f>IF(B140 = Fases!$A$2,Tabela2[[#This Row],[Tempo gasto]],0)</f>
@@ -3415,7 +3424,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="141" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="141" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C141" s="5"/>
       <c r="D141" s="2">
         <f>IF(B141 = Fases!$A$2,Tabela2[[#This Row],[Tempo gasto]],0)</f>
@@ -3430,7 +3439,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="142" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="142" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C142" s="5"/>
       <c r="D142" s="2">
         <f>IF(B142 = Fases!$A$2,Tabela2[[#This Row],[Tempo gasto]],0)</f>
@@ -3445,7 +3454,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="143" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="143" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C143" s="5"/>
       <c r="D143" s="2">
         <f>IF(B143 = Fases!$A$2,Tabela2[[#This Row],[Tempo gasto]],0)</f>
@@ -3460,7 +3469,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="144" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="144" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C144" s="5"/>
       <c r="D144" s="2">
         <f>IF(B144 = Fases!$A$2,Tabela2[[#This Row],[Tempo gasto]],0)</f>
@@ -3475,7 +3484,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="145" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="145" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C145" s="5"/>
       <c r="D145" s="2">
         <f>IF(B145 = Fases!$A$2,Tabela2[[#This Row],[Tempo gasto]],0)</f>
@@ -3490,7 +3499,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="146" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="146" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C146" s="5"/>
       <c r="D146" s="2">
         <f>IF(B146 = Fases!$A$2,Tabela2[[#This Row],[Tempo gasto]],0)</f>
@@ -3505,7 +3514,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="147" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="147" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C147" s="5"/>
       <c r="D147" s="2">
         <f>IF(B147 = Fases!$A$2,Tabela2[[#This Row],[Tempo gasto]],0)</f>
@@ -3520,7 +3529,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="148" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="148" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C148" s="5"/>
       <c r="D148" s="2">
         <f>IF(B148 = Fases!$A$2,Tabela2[[#This Row],[Tempo gasto]],0)</f>
@@ -3535,7 +3544,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="149" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="149" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C149" s="5"/>
       <c r="D149" s="2">
         <f>IF(B149 = Fases!$A$2,Tabela2[[#This Row],[Tempo gasto]],0)</f>
@@ -3550,7 +3559,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="150" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="150" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C150" s="5"/>
       <c r="D150" s="2">
         <f>IF(B150 = Fases!$A$2,Tabela2[[#This Row],[Tempo gasto]],0)</f>
@@ -3565,7 +3574,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="151" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="151" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C151" s="5"/>
       <c r="D151" s="2">
         <f>IF(B151 = Fases!$A$2,Tabela2[[#This Row],[Tempo gasto]],0)</f>
@@ -3580,7 +3589,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="152" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="152" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C152" s="5"/>
       <c r="D152" s="2">
         <f>IF(B152 = Fases!$A$2,Tabela2[[#This Row],[Tempo gasto]],0)</f>
@@ -3595,7 +3604,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="153" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="153" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C153" s="5"/>
       <c r="D153" s="2">
         <f>IF(B153 = Fases!$A$2,Tabela2[[#This Row],[Tempo gasto]],0)</f>
@@ -3610,7 +3619,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="154" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="154" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C154" s="5"/>
       <c r="D154" s="2">
         <f>IF(B154 = Fases!$A$2,Tabela2[[#This Row],[Tempo gasto]],0)</f>
@@ -3625,7 +3634,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="155" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="155" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C155" s="5"/>
       <c r="D155" s="2">
         <f>IF(B155 = Fases!$A$2,Tabela2[[#This Row],[Tempo gasto]],0)</f>
@@ -3640,7 +3649,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="156" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="156" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C156" s="5"/>
       <c r="D156" s="2">
         <f>IF(B156 = Fases!$A$2,Tabela2[[#This Row],[Tempo gasto]],0)</f>
@@ -3655,7 +3664,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="157" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="157" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C157" s="5"/>
       <c r="D157" s="2">
         <f>IF(B157 = Fases!$A$2,Tabela2[[#This Row],[Tempo gasto]],0)</f>
@@ -3670,7 +3679,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="158" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="158" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C158" s="5"/>
       <c r="D158" s="2">
         <f>IF(B158 = Fases!$A$2,Tabela2[[#This Row],[Tempo gasto]],0)</f>
@@ -3685,7 +3694,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="159" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="159" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C159" s="5"/>
       <c r="D159" s="2">
         <f>IF(B159 = Fases!$A$2,Tabela2[[#This Row],[Tempo gasto]],0)</f>
@@ -3700,7 +3709,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="160" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="160" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C160" s="5"/>
       <c r="D160" s="2">
         <f>IF(B160 = Fases!$A$2,Tabela2[[#This Row],[Tempo gasto]],0)</f>
@@ -3715,7 +3724,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="161" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="161" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C161" s="5"/>
       <c r="D161" s="2">
         <f>IF(B161 = Fases!$A$2,Tabela2[[#This Row],[Tempo gasto]],0)</f>
@@ -3730,7 +3739,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="162" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="162" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C162" s="5"/>
       <c r="D162" s="2">
         <f>IF(B162 = Fases!$A$2,Tabela2[[#This Row],[Tempo gasto]],0)</f>
@@ -3745,7 +3754,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="163" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="163" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C163" s="5"/>
       <c r="D163" s="2">
         <f>IF(B163 = Fases!$A$2,Tabela2[[#This Row],[Tempo gasto]],0)</f>
@@ -3760,7 +3769,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="164" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="164" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C164" s="5"/>
       <c r="D164" s="2">
         <f>IF(B164 = Fases!$A$2,Tabela2[[#This Row],[Tempo gasto]],0)</f>
@@ -3775,7 +3784,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="165" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="165" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C165" s="5"/>
       <c r="D165" s="2">
         <f>IF(B165 = Fases!$A$2,Tabela2[[#This Row],[Tempo gasto]],0)</f>
@@ -3790,7 +3799,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="166" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="166" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C166" s="5"/>
       <c r="D166" s="2">
         <f>IF(B166 = Fases!$A$2,Tabela2[[#This Row],[Tempo gasto]],0)</f>
@@ -3805,7 +3814,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="167" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="167" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C167" s="5"/>
       <c r="D167" s="2">
         <f>IF(B167 = Fases!$A$2,Tabela2[[#This Row],[Tempo gasto]],0)</f>
@@ -3820,7 +3829,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="168" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="168" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C168" s="5"/>
       <c r="D168" s="2">
         <f>IF(B168 = Fases!$A$2,Tabela2[[#This Row],[Tempo gasto]],0)</f>
@@ -3835,7 +3844,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="169" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="169" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C169" s="5"/>
       <c r="D169" s="2">
         <f>IF(B169 = Fases!$A$2,Tabela2[[#This Row],[Tempo gasto]],0)</f>
@@ -3850,7 +3859,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="170" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="170" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C170" s="5"/>
       <c r="D170" s="2">
         <f>IF(B170 = Fases!$A$2,Tabela2[[#This Row],[Tempo gasto]],0)</f>
@@ -3865,7 +3874,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="171" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="171" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C171" s="5"/>
       <c r="D171" s="2">
         <f>IF(B171 = Fases!$A$2,Tabela2[[#This Row],[Tempo gasto]],0)</f>
@@ -3880,7 +3889,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="172" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="172" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C172" s="5"/>
       <c r="D172" s="2">
         <f>IF(B172 = Fases!$A$2,Tabela2[[#This Row],[Tempo gasto]],0)</f>
@@ -3895,7 +3904,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="173" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="173" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C173" s="5"/>
       <c r="D173" s="2">
         <f>IF(B173 = Fases!$A$2,Tabela2[[#This Row],[Tempo gasto]],0)</f>
@@ -3910,7 +3919,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="174" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="174" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C174" s="5"/>
       <c r="D174" s="2">
         <f>IF(B174 = Fases!$A$2,Tabela2[[#This Row],[Tempo gasto]],0)</f>
@@ -3925,7 +3934,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="175" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="175" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C175" s="5"/>
       <c r="D175" s="2">
         <f>IF(B175 = Fases!$A$2,Tabela2[[#This Row],[Tempo gasto]],0)</f>
@@ -3940,7 +3949,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="176" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="176" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C176" s="5"/>
       <c r="D176" s="2">
         <f>IF(B176 = Fases!$A$2,Tabela2[[#This Row],[Tempo gasto]],0)</f>
@@ -3955,7 +3964,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="177" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="177" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C177" s="5"/>
       <c r="D177" s="2">
         <f>IF(B177 = Fases!$A$2,Tabela2[[#This Row],[Tempo gasto]],0)</f>
@@ -3970,7 +3979,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="178" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="178" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C178" s="5"/>
       <c r="D178" s="2">
         <f>IF(B178 = Fases!$A$2,Tabela2[[#This Row],[Tempo gasto]],0)</f>
@@ -3985,7 +3994,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="179" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="179" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C179" s="5"/>
       <c r="D179" s="2">
         <f>IF(B179 = Fases!$A$2,Tabela2[[#This Row],[Tempo gasto]],0)</f>
@@ -4000,7 +4009,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="180" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="180" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C180" s="5"/>
       <c r="D180" s="2">
         <f>IF(B180 = Fases!$A$2,Tabela2[[#This Row],[Tempo gasto]],0)</f>
@@ -4015,7 +4024,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="181" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="181" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C181" s="5"/>
       <c r="D181" s="2">
         <f>IF(B181 = Fases!$A$2,Tabela2[[#This Row],[Tempo gasto]],0)</f>
@@ -4030,7 +4039,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="182" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="182" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C182" s="5"/>
       <c r="D182" s="2">
         <f>IF(B182 = Fases!$A$2,Tabela2[[#This Row],[Tempo gasto]],0)</f>
@@ -4045,7 +4054,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="183" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="183" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C183" s="5"/>
       <c r="D183" s="2">
         <f>IF(B183 = Fases!$A$2,Tabela2[[#This Row],[Tempo gasto]],0)</f>
@@ -4060,7 +4069,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="184" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="184" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C184" s="5"/>
       <c r="D184" s="2">
         <f>IF(B184 = Fases!$A$2,Tabela2[[#This Row],[Tempo gasto]],0)</f>
@@ -4075,7 +4084,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="185" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="185" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C185" s="5"/>
       <c r="D185" s="2">
         <f>IF(B185 = Fases!$A$2,Tabela2[[#This Row],[Tempo gasto]],0)</f>
@@ -4090,7 +4099,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="186" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="186" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C186" s="5"/>
       <c r="D186" s="2">
         <f>IF(B186 = Fases!$A$2,Tabela2[[#This Row],[Tempo gasto]],0)</f>
@@ -4105,7 +4114,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="187" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="187" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C187" s="5"/>
       <c r="D187" s="2">
         <f>IF(B187 = Fases!$A$2,Tabela2[[#This Row],[Tempo gasto]],0)</f>
@@ -4120,7 +4129,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="188" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="188" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C188" s="5"/>
       <c r="D188" s="2">
         <f>IF(B188 = Fases!$A$2,Tabela2[[#This Row],[Tempo gasto]],0)</f>
@@ -4135,7 +4144,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="189" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="189" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C189" s="5"/>
       <c r="D189" s="2">
         <f>IF(B189 = Fases!$A$2,Tabela2[[#This Row],[Tempo gasto]],0)</f>
@@ -4150,7 +4159,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="190" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="190" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C190" s="5"/>
       <c r="D190" s="2">
         <f>IF(B190 = Fases!$A$2,Tabela2[[#This Row],[Tempo gasto]],0)</f>
@@ -4165,7 +4174,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="191" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="191" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C191" s="5"/>
       <c r="D191" s="2">
         <f>IF(B191 = Fases!$A$2,Tabela2[[#This Row],[Tempo gasto]],0)</f>
@@ -4180,7 +4189,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="192" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="192" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C192" s="5"/>
       <c r="D192" s="2">
         <f>IF(B192 = Fases!$A$2,Tabela2[[#This Row],[Tempo gasto]],0)</f>
@@ -4195,7 +4204,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="193" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="193" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C193" s="5"/>
       <c r="D193" s="2">
         <f>IF(B193 = Fases!$A$2,Tabela2[[#This Row],[Tempo gasto]],0)</f>
@@ -4210,7 +4219,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="194" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="194" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C194" s="5"/>
       <c r="D194" s="2">
         <f>IF(B194 = Fases!$A$2,Tabela2[[#This Row],[Tempo gasto]],0)</f>
@@ -4225,7 +4234,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="195" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="195" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C195" s="5"/>
       <c r="D195" s="2">
         <f>IF(B195 = Fases!$A$2,Tabela2[[#This Row],[Tempo gasto]],0)</f>
@@ -4240,7 +4249,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="196" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="196" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C196" s="5"/>
       <c r="D196" s="2">
         <f>IF(B196 = Fases!$A$2,Tabela2[[#This Row],[Tempo gasto]],0)</f>
@@ -4255,7 +4264,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="197" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="197" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C197" s="5"/>
       <c r="D197" s="2">
         <f>IF(B197 = Fases!$A$2,Tabela2[[#This Row],[Tempo gasto]],0)</f>
@@ -4270,7 +4279,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="198" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="198" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C198" s="5"/>
       <c r="D198" s="2">
         <f>IF(B198 = Fases!$A$2,Tabela2[[#This Row],[Tempo gasto]],0)</f>
@@ -4285,7 +4294,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="199" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="199" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C199" s="5"/>
       <c r="D199" s="2">
         <f>IF(B199 = Fases!$A$2,Tabela2[[#This Row],[Tempo gasto]],0)</f>
@@ -4300,7 +4309,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="200" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="200" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C200" s="5"/>
       <c r="D200" s="2">
         <f>IF(B200 = Fases!$A$2,Tabela2[[#This Row],[Tempo gasto]],0)</f>
@@ -4315,7 +4324,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="201" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="201" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C201" s="5"/>
       <c r="D201" s="2">
         <f>IF(B201 = Fases!$A$2,Tabela2[[#This Row],[Tempo gasto]],0)</f>
@@ -4330,7 +4339,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="202" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="202" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C202" s="5"/>
       <c r="D202" s="2">
         <f>IF(B202 = Fases!$A$2,Tabela2[[#This Row],[Tempo gasto]],0)</f>
@@ -4345,7 +4354,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="203" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="203" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C203" s="5"/>
       <c r="D203" s="2">
         <f>IF(B203 = Fases!$A$2,Tabela2[[#This Row],[Tempo gasto]],0)</f>
@@ -4360,7 +4369,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="204" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="204" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C204" s="5"/>
       <c r="D204" s="2">
         <f>IF(B204 = Fases!$A$2,Tabela2[[#This Row],[Tempo gasto]],0)</f>
@@ -4375,7 +4384,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="205" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="205" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C205" s="5"/>
       <c r="D205" s="2">
         <f>IF(B205 = Fases!$A$2,Tabela2[[#This Row],[Tempo gasto]],0)</f>
@@ -4390,7 +4399,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="206" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="206" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C206" s="5"/>
       <c r="D206" s="2">
         <f>IF(B206 = Fases!$A$2,Tabela2[[#This Row],[Tempo gasto]],0)</f>
@@ -4405,7 +4414,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="207" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="207" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C207" s="5"/>
       <c r="D207" s="2">
         <f>IF(B207 = Fases!$A$2,Tabela2[[#This Row],[Tempo gasto]],0)</f>
@@ -4420,7 +4429,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="208" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="208" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C208" s="5"/>
       <c r="D208" s="2">
         <f>IF(B208 = Fases!$A$2,Tabela2[[#This Row],[Tempo gasto]],0)</f>
@@ -4435,7 +4444,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="209" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="209" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C209" s="5"/>
       <c r="D209" s="2">
         <f>IF(B209 = Fases!$A$2,Tabela2[[#This Row],[Tempo gasto]],0)</f>
@@ -4450,7 +4459,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="210" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="210" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C210" s="5"/>
       <c r="D210" s="2">
         <f>IF(B210 = Fases!$A$2,Tabela2[[#This Row],[Tempo gasto]],0)</f>
@@ -4465,7 +4474,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="211" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="211" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C211" s="5"/>
       <c r="D211" s="2">
         <f>IF(B211 = Fases!$A$2,Tabela2[[#This Row],[Tempo gasto]],0)</f>
@@ -4480,7 +4489,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="212" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="212" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C212" s="5"/>
       <c r="D212" s="2">
         <f>IF(B212 = Fases!$A$2,Tabela2[[#This Row],[Tempo gasto]],0)</f>
@@ -4495,7 +4504,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="213" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="213" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C213" s="5"/>
       <c r="D213" s="2">
         <f>IF(B213 = Fases!$A$2,Tabela2[[#This Row],[Tempo gasto]],0)</f>
@@ -4510,7 +4519,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="214" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="214" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C214" s="5"/>
       <c r="D214" s="2">
         <f>IF(B214 = Fases!$A$2,Tabela2[[#This Row],[Tempo gasto]],0)</f>
@@ -4525,7 +4534,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="215" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="215" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C215" s="5"/>
       <c r="D215" s="2">
         <f>IF(B215 = Fases!$A$2,Tabela2[[#This Row],[Tempo gasto]],0)</f>
@@ -4540,7 +4549,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="216" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="216" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C216" s="5"/>
       <c r="D216" s="2">
         <f>IF(B216 = Fases!$A$2,Tabela2[[#This Row],[Tempo gasto]],0)</f>
@@ -4555,7 +4564,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="217" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="217" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C217" s="5"/>
       <c r="D217" s="2">
         <f>IF(B217 = Fases!$A$2,Tabela2[[#This Row],[Tempo gasto]],0)</f>
@@ -4570,7 +4579,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="218" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="218" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C218" s="5"/>
       <c r="D218" s="2">
         <f>IF(B218 = Fases!$A$2,Tabela2[[#This Row],[Tempo gasto]],0)</f>
@@ -4585,7 +4594,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="219" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="219" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C219" s="5"/>
       <c r="D219" s="2">
         <f>IF(B219 = Fases!$A$2,Tabela2[[#This Row],[Tempo gasto]],0)</f>
@@ -4600,7 +4609,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="220" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="220" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C220" s="5"/>
       <c r="D220" s="2">
         <f>IF(B220 = Fases!$A$2,Tabela2[[#This Row],[Tempo gasto]],0)</f>
@@ -4615,7 +4624,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="221" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="221" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C221" s="5"/>
       <c r="D221" s="2">
         <f>IF(B221 = Fases!$A$2,Tabela2[[#This Row],[Tempo gasto]],0)</f>
@@ -4630,7 +4639,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="222" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="222" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C222" s="5"/>
       <c r="D222" s="2">
         <f>IF(B222 = Fases!$A$2,Tabela2[[#This Row],[Tempo gasto]],0)</f>
@@ -4645,7 +4654,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="223" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="223" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C223" s="5"/>
       <c r="D223" s="2">
         <f>IF(B223 = Fases!$A$2,Tabela2[[#This Row],[Tempo gasto]],0)</f>
@@ -4660,7 +4669,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="224" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="224" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C224" s="5"/>
       <c r="D224" s="2">
         <f>IF(B224 = Fases!$A$2,Tabela2[[#This Row],[Tempo gasto]],0)</f>
@@ -4675,7 +4684,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="225" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="225" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C225" s="5"/>
       <c r="D225" s="2">
         <f>IF(B225 = Fases!$A$2,Tabela2[[#This Row],[Tempo gasto]],0)</f>
@@ -4690,7 +4699,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="226" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="226" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C226" s="5"/>
       <c r="D226" s="2">
         <f>IF(B226 = Fases!$A$2,Tabela2[[#This Row],[Tempo gasto]],0)</f>
@@ -4705,7 +4714,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="227" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="227" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C227" s="5"/>
       <c r="D227" s="2">
         <f>IF(B227 = Fases!$A$2,Tabela2[[#This Row],[Tempo gasto]],0)</f>
@@ -4720,7 +4729,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="228" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="228" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C228" s="5"/>
       <c r="D228" s="2">
         <f>IF(B228 = Fases!$A$2,Tabela2[[#This Row],[Tempo gasto]],0)</f>
@@ -4735,7 +4744,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="229" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="229" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C229" s="5"/>
       <c r="D229" s="2">
         <f>IF(B229 = Fases!$A$2,Tabela2[[#This Row],[Tempo gasto]],0)</f>
@@ -4750,7 +4759,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="230" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="230" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C230" s="5"/>
       <c r="D230" s="2">
         <f>IF(B230 = Fases!$A$2,Tabela2[[#This Row],[Tempo gasto]],0)</f>
@@ -4765,7 +4774,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="231" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="231" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C231" s="5"/>
       <c r="D231" s="2">
         <f>IF(B231 = Fases!$A$2,Tabela2[[#This Row],[Tempo gasto]],0)</f>
@@ -4780,7 +4789,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="232" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="232" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C232" s="5"/>
       <c r="D232" s="2">
         <f>IF(B232 = Fases!$A$2,Tabela2[[#This Row],[Tempo gasto]],0)</f>
@@ -4795,7 +4804,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="233" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="233" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C233" s="5"/>
       <c r="D233" s="2">
         <f>IF(B233 = Fases!$A$2,Tabela2[[#This Row],[Tempo gasto]],0)</f>
@@ -4810,7 +4819,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="234" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="234" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C234" s="5"/>
       <c r="D234" s="2">
         <f>IF(B234 = Fases!$A$2,Tabela2[[#This Row],[Tempo gasto]],0)</f>
@@ -4825,7 +4834,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="235" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="235" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C235" s="5"/>
       <c r="D235" s="2">
         <f>IF(B235 = Fases!$A$2,Tabela2[[#This Row],[Tempo gasto]],0)</f>
@@ -4840,7 +4849,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="236" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="236" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C236" s="5"/>
       <c r="D236" s="2">
         <f>IF(B236 = Fases!$A$2,Tabela2[[#This Row],[Tempo gasto]],0)</f>
@@ -4855,7 +4864,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="237" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="237" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C237" s="5"/>
       <c r="D237" s="2">
         <f>IF(B237 = Fases!$A$2,Tabela2[[#This Row],[Tempo gasto]],0)</f>
@@ -4870,7 +4879,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="238" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="238" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C238" s="5"/>
       <c r="D238" s="2">
         <f>IF(B238 = Fases!$A$2,Tabela2[[#This Row],[Tempo gasto]],0)</f>
@@ -4885,7 +4894,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="239" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="239" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C239" s="5"/>
       <c r="D239" s="2">
         <f>IF(B239 = Fases!$A$2,Tabela2[[#This Row],[Tempo gasto]],0)</f>
@@ -4900,7 +4909,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="240" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="240" spans="3:6" x14ac:dyDescent="0.35">
       <c r="C240" s="5"/>
       <c r="D240" s="2">
         <f>IF(B240 = Fases!$A$2,Tabela2[[#This Row],[Tempo gasto]],0)</f>
@@ -4915,7 +4924,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="241" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="241" spans="1:6" x14ac:dyDescent="0.35">
       <c r="C241" s="5"/>
       <c r="D241" s="2">
         <f>IF(B241 = Fases!$A$2,Tabela2[[#This Row],[Tempo gasto]],0)</f>
@@ -4930,7 +4939,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="242" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="242" spans="1:6" x14ac:dyDescent="0.35">
       <c r="C242" s="5"/>
       <c r="D242" s="2">
         <f>IF(B242 = Fases!$A$2,Tabela2[[#This Row],[Tempo gasto]],0)</f>
@@ -4945,7 +4954,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="243" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="243" spans="1:6" x14ac:dyDescent="0.35">
       <c r="C243" s="5"/>
       <c r="D243" s="2">
         <f>IF(B243 = Fases!$A$2,Tabela2[[#This Row],[Tempo gasto]],0)</f>
@@ -4960,7 +4969,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="244" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="244" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A244" s="9"/>
       <c r="B244" s="10"/>
       <c r="C244" s="11"/>
@@ -4970,7 +4979,7 @@
       </c>
       <c r="E244" s="12">
         <f>SUBTOTAL(109,Tabela2[Consolidado fase 2])</f>
-        <v>0.35</v>
+        <v>0.41249999999999998</v>
       </c>
       <c r="F244" s="12">
         <f>SUBTOTAL(109,Tabela2[Consolidado fase 3])</f>
@@ -5022,12 +5031,12 @@
       <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="47.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -5035,7 +5044,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>15</v>
       </c>
@@ -5043,7 +5052,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>17</v>
       </c>
@@ -5051,7 +5060,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>18</v>
       </c>

</xml_diff>

<commit_message>
Controle de Tempo + Imagem
</commit_message>
<xml_diff>
--- a/Controle-de-tempo.xlsx
+++ b/Controle-de-tempo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/16d1df2b2646901a/Documentos/GitHub/Automatizacao/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="3" documentId="13_ncr:1_{4E50F906-144F-594E-B99D-9BAD18E2584F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5BCFD88C-C264-444B-9C5A-98EB1A116161}"/>
+  <xr:revisionPtr revIDLastSave="6" documentId="13_ncr:1_{4E50F906-144F-594E-B99D-9BAD18E2584F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BC55FF0A-974F-44D7-8D64-8BC92E7EB776}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{3FD58BC0-7166-A544-9D3F-4C0C6ADD0B8E}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="19">
   <si>
     <t>Programador</t>
   </si>
@@ -1039,8 +1039,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3BA28EEB-0D8A-B34C-A5FE-30F0F9165161}">
   <dimension ref="A1:O244"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -1235,7 +1235,7 @@
       </c>
       <c r="J5" s="14">
         <f>E244</f>
-        <v>0.41249999999999998</v>
+        <v>0.47499999999999998</v>
       </c>
       <c r="K5" s="14">
         <f>Tabela3[[#This Row],[Total Estimado]]/2</f>
@@ -1243,7 +1243,7 @@
       </c>
       <c r="L5" s="14">
         <f>SUMIFS($C$2:$C$200,$B$2:$B$200,"Semana 2",$A$2:$A$200,"Cesar")</f>
-        <v>0.16666666666666666</v>
+        <v>0.22916666666666666</v>
       </c>
       <c r="M5" s="14">
         <f>Tabela3[[#This Row],[Total Estimado]]/2</f>
@@ -1255,7 +1255,7 @@
       </c>
       <c r="O5" s="14">
         <f t="shared" ref="O5:O6" si="0">I5 - J5</f>
-        <v>0.42083333333333339</v>
+        <v>0.35833333333333339</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.35">
@@ -1593,15 +1593,22 @@
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="B19" s="4"/>
-      <c r="C19" s="5"/>
+      <c r="A19" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C19" s="5">
+        <v>6.25E-2</v>
+      </c>
       <c r="D19" s="2">
         <f>IF(B19 = Fases!$A$2,Tabela2[[#This Row],[Tempo gasto]],0)</f>
         <v>0</v>
       </c>
       <c r="E19" s="2">
         <f>IF(B19 = Fases!$A$3,Tabela2[[#This Row],[Tempo gasto]],0)</f>
-        <v>0</v>
+        <v>6.25E-2</v>
       </c>
       <c r="F19" s="7">
         <f>IF(B19 = Fases!$A$4,Tabela2[[#This Row],[Tempo gasto]],0)</f>
@@ -4979,7 +4986,7 @@
       </c>
       <c r="E244" s="12">
         <f>SUBTOTAL(109,Tabela2[Consolidado fase 2])</f>
-        <v>0.41249999999999998</v>
+        <v>0.47499999999999998</v>
       </c>
       <c r="F244" s="12">
         <f>SUBTOTAL(109,Tabela2[Consolidado fase 3])</f>

</xml_diff>

<commit_message>
Lançando as horas do Catulo
</commit_message>
<xml_diff>
--- a/Controle-de-tempo.xlsx
+++ b/Controle-de-tempo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/leonardoamaral/Documents/GitHub/Automatizacao/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{970D3780-E8E3-6B4D-BC72-93EE95111D55}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06629579-C390-E24A-B435-2F6FD4E1374D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="17140" xr2:uid="{3FD58BC0-7166-A544-9D3F-4C0C6ADD0B8E}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="19">
   <si>
     <t>Programador</t>
   </si>
@@ -1038,7 +1038,7 @@
   <dimension ref="A1:O244"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C32" sqref="C32"/>
+      <selection activeCell="G34" sqref="G34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1286,7 +1286,7 @@
       </c>
       <c r="J6" s="14">
         <f t="shared" ref="J6" si="1">F244</f>
-        <v>0.26319444444444445</v>
+        <v>0.40902777777777777</v>
       </c>
       <c r="K6" s="16">
         <f>Tabela3[[#This Row],[Total Estimado]]/2</f>
@@ -1294,7 +1294,7 @@
       </c>
       <c r="L6" s="16">
         <f>SUMIFS($C$2:$C$200,$B$2:$B$200,"Semana 3",$A$2:$A$200,"Cesar")</f>
-        <v>4.8611111111111112E-2</v>
+        <v>0.19444444444444445</v>
       </c>
       <c r="M6" s="17">
         <f>Tabela3[[#This Row],[Total Estimado]]/2</f>
@@ -1306,7 +1306,7 @@
       </c>
       <c r="O6" s="14">
         <f t="shared" si="0"/>
-        <v>0.57013888888888897</v>
+        <v>0.4243055555555556</v>
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.2">
@@ -1890,7 +1890,15 @@
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="C32" s="5"/>
+      <c r="A32" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B32" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C32" s="5">
+        <v>8.3333333333333329E-2</v>
+      </c>
       <c r="D32" s="2">
         <f>IF(B32 = Fases!$A$2,Tabela2[[#This Row],[Tempo gasto]],0)</f>
         <v>0</v>
@@ -1901,11 +1909,19 @@
       </c>
       <c r="F32" s="7">
         <f>IF(B32 = Fases!$A$4,Tabela2[[#This Row],[Tempo gasto]],0)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="33" spans="3:6" x14ac:dyDescent="0.2">
-      <c r="C33" s="5"/>
+        <v>8.3333333333333329E-2</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A33" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B33" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C33" s="5">
+        <v>6.25E-2</v>
+      </c>
       <c r="D33" s="2">
         <f>IF(B33 = Fases!$A$2,Tabela2[[#This Row],[Tempo gasto]],0)</f>
         <v>0</v>
@@ -1916,10 +1932,10 @@
       </c>
       <c r="F33" s="7">
         <f>IF(B33 = Fases!$A$4,Tabela2[[#This Row],[Tempo gasto]],0)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="34" spans="3:6" x14ac:dyDescent="0.2">
+        <v>6.25E-2</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
       <c r="C34" s="5"/>
       <c r="D34" s="2">
         <f>IF(B34 = Fases!$A$2,Tabela2[[#This Row],[Tempo gasto]],0)</f>
@@ -1934,7 +1950,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
       <c r="C35" s="5"/>
       <c r="D35" s="2">
         <f>IF(B35 = Fases!$A$2,Tabela2[[#This Row],[Tempo gasto]],0)</f>
@@ -1949,7 +1965,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
       <c r="C36" s="5"/>
       <c r="D36" s="2">
         <f>IF(B36 = Fases!$A$2,Tabela2[[#This Row],[Tempo gasto]],0)</f>
@@ -1964,7 +1980,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
       <c r="C37" s="5"/>
       <c r="D37" s="2">
         <f>IF(B37 = Fases!$A$2,Tabela2[[#This Row],[Tempo gasto]],0)</f>
@@ -1979,7 +1995,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
       <c r="C38" s="5"/>
       <c r="D38" s="2">
         <f>IF(B38 = Fases!$A$2,Tabela2[[#This Row],[Tempo gasto]],0)</f>
@@ -1994,7 +2010,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
       <c r="C39" s="5"/>
       <c r="D39" s="2">
         <f>IF(B39 = Fases!$A$2,Tabela2[[#This Row],[Tempo gasto]],0)</f>
@@ -2009,7 +2025,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
       <c r="C40" s="5"/>
       <c r="D40" s="2">
         <f>IF(B40 = Fases!$A$2,Tabela2[[#This Row],[Tempo gasto]],0)</f>
@@ -2024,7 +2040,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
       <c r="C41" s="5"/>
       <c r="D41" s="2">
         <f>IF(B41 = Fases!$A$2,Tabela2[[#This Row],[Tempo gasto]],0)</f>
@@ -2039,7 +2055,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
       <c r="C42" s="5"/>
       <c r="D42" s="2">
         <f>IF(B42 = Fases!$A$2,Tabela2[[#This Row],[Tempo gasto]],0)</f>
@@ -2054,7 +2070,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
       <c r="C43" s="5"/>
       <c r="D43" s="2">
         <f>IF(B43 = Fases!$A$2,Tabela2[[#This Row],[Tempo gasto]],0)</f>
@@ -2069,7 +2085,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
       <c r="C44" s="5"/>
       <c r="D44" s="2">
         <f>IF(B44 = Fases!$A$2,Tabela2[[#This Row],[Tempo gasto]],0)</f>
@@ -2084,7 +2100,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
       <c r="C45" s="5"/>
       <c r="D45" s="2">
         <f>IF(B45 = Fases!$A$2,Tabela2[[#This Row],[Tempo gasto]],0)</f>
@@ -2099,7 +2115,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
       <c r="C46" s="5"/>
       <c r="D46" s="2">
         <f>IF(B46 = Fases!$A$2,Tabela2[[#This Row],[Tempo gasto]],0)</f>
@@ -2114,7 +2130,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
       <c r="C47" s="5"/>
       <c r="D47" s="2">
         <f>IF(B47 = Fases!$A$2,Tabela2[[#This Row],[Tempo gasto]],0)</f>
@@ -2129,7 +2145,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="3:6" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
       <c r="C48" s="5"/>
       <c r="D48" s="2">
         <f>IF(B48 = Fases!$A$2,Tabela2[[#This Row],[Tempo gasto]],0)</f>
@@ -5083,7 +5099,7 @@
       </c>
       <c r="F244" s="12">
         <f>SUBTOTAL(109,Tabela2[Consolidado fase 3])</f>
-        <v>0.26319444444444445</v>
+        <v>0.40902777777777777</v>
       </c>
     </row>
   </sheetData>

</xml_diff>